<commit_message>
created class to read data from excel
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82C3500D-C260-41C3-B60A-7A178ED5F7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F29ECE3-8CA4-42E2-A7E8-5C0AE95C993D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="3348" yWindow="3900" windowWidth="17280" windowHeight="9960" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H13:H14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added you Cart and Your information class. Added test methods for your Cart and your Information.
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lolo.Nkosi\Documents\PROJECT\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622351DC-8B3B-49BD-962E-A7EBCB6B1092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC60AF8-FB28-419A-B8FE-C3A861B1F906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="3240" windowWidth="17280" windowHeight="9960" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="35625" yWindow="1650" windowWidth="14400" windowHeight="7275" firstSheet="1" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>secret_sauce1</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name </t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>2194</t>
   </si>
 </sst>
 </file>
@@ -94,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +128,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,10 +171,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,17 +523,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC3EE8-0C30-457B-B4C6-250A2CD71A8D}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -507,7 +549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -515,7 +557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -523,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -531,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -539,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -547,39 +589,39 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -590,14 +632,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110EF415-BA76-4F5F-B1DB-7BD8BBD114F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created extent reports and listener methods.
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Precious\Videos\Automation class session\ProjectFramework\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19373893-E0D0-4FB0-8679-C2E80A0E48BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABC697A-4A91-4EAD-A894-3E8F79CDBBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17EF97C6-4FC7-4A7E-95B6-049C22C9243A}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{17EF97C6-4FC7-4A7E-95B6-049C22C9243A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>PN</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2BB328-4E32-42CE-9F23-C1D9CCC909D5}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -569,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26C98FE-5D15-466C-ABF9-247C46E5E962}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,8 +605,8 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1687</v>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ReadFromExcel.javaclass, excel data and purchaseItemTests.java. Also pom file to add dependencies
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eoh-my.sharepoint.com/personal/anna_pohotona_eoh_co_za/Documents/Projects/SauceDemo2ndGroup2025/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622351DC-8B3B-49BD-962E-A7EBCB6B1092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{12D2C31D-84F4-4DE0-A4FA-3EEA5CDA18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="3240" windowWidth="17280" windowHeight="9960" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>secret_sauce1</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>Molatelo</t>
+  </si>
+  <si>
+    <t>Pohotona</t>
   </si>
 </sst>
 </file>
@@ -94,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,10 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC3EE8-0C30-457B-B4C6-250A2CD71A8D}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -590,14 +615,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110EF415-BA76-4F5F-B1DB-7BD8BBD114F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1459</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assesment 2025/04/02 till Checkout: Overview
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lebogang.maepa\Downloads\Thabiso Automation\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622351DC-8B3B-49BD-962E-A7EBCB6B1092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E40F57-B034-454E-BD63-0E6F8C51F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="3240" windowWidth="17280" windowHeight="9960" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>secret_sauce1</t>
+  </si>
+  <si>
+    <t>Thabiso</t>
+  </si>
+  <si>
+    <t>Ndlovu</t>
+  </si>
+  <si>
+    <t>postalcode</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -481,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC3EE8-0C30-457B-B4C6-250A2CD71A8D}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,14 +611,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110EF415-BA76-4F5F-B1DB-7BD8BBD114F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>7441</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2 more pages and edited the code so that we can verify the correct price is displayed
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lotha\OneDrive\Documents\Java Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622351DC-8B3B-49BD-962E-A7EBCB6B1092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58027C03-3FB7-492D-97FA-E1D7A11A3FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="3240" windowWidth="17280" windowHeight="9960" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>secret_sauce1</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Lothando</t>
+  </si>
+  <si>
+    <t>Khumalo</t>
+  </si>
+  <si>
+    <t>Thando</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
   </si>
 </sst>
 </file>
@@ -481,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC3EE8-0C30-457B-B4C6-250A2CD71A8D}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,19 +603,59 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110EF415-BA76-4F5F-B1DB-7BD8BBD114F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2091</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add items,verify cart items and screenshots
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masha\Documents\Projects\SauceDemo2ndGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19613064-490A-434F-B3FB-71F27CB7DE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEFE456-C8DC-4B67-B5D6-DD8F982BFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9029EFAD-4DF3-4B15-AA2E-50BF92F45BC4}"/>
   </bookViews>
@@ -176,14 +176,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +630,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +646,7 @@
       <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -659,7 +657,7 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="3">
         <v>182</v>
       </c>
     </row>
@@ -670,7 +668,7 @@
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>9861</v>
       </c>
     </row>
@@ -681,69 +679,69 @@
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>1256</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>